<commit_message>
ajustando rotas para leitura do arquivo
</commit_message>
<xml_diff>
--- a/confirmation.xlsx
+++ b/confirmation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newma\Documents\casamento\convite-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65F655A-43D4-48C1-AF86-1967B38503FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D07085-86C6-430D-80FF-3076FF2D95B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15150" yWindow="630" windowWidth="20520" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16065" yWindow="375" windowWidth="20520" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
   <si>
     <t>Maria Pereira</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Débora Pereira</t>
   </si>
   <si>
-    <t>Daniel, Bia, Namorado Bia</t>
-  </si>
-  <si>
     <t>Karol</t>
   </si>
   <si>
@@ -112,15 +109,9 @@
     <t>Tom</t>
   </si>
   <si>
-    <t>Bruna, Filhos</t>
-  </si>
-  <si>
     <t>Oseias Pereira</t>
   </si>
   <si>
-    <t>Daiana, Davi</t>
-  </si>
-  <si>
     <t>Joana Escobar</t>
   </si>
   <si>
@@ -142,9 +133,6 @@
     <t>Maria</t>
   </si>
   <si>
-    <t>Cauã, Namorada</t>
-  </si>
-  <si>
     <t>João</t>
   </si>
   <si>
@@ -160,21 +148,12 @@
     <t>Rosemiro</t>
   </si>
   <si>
-    <t>Idalina, 4</t>
-  </si>
-  <si>
     <t>Rosa</t>
   </si>
   <si>
-    <t>Celio, Dois Filhos</t>
-  </si>
-  <si>
     <t>Luciana</t>
   </si>
   <si>
-    <t>José Zito, 3 filhos</t>
-  </si>
-  <si>
     <t>Roberto</t>
   </si>
   <si>
@@ -238,9 +217,6 @@
     <t>Marcos</t>
   </si>
   <si>
-    <t>Marinalva, 3 filhos</t>
-  </si>
-  <si>
     <t>Julia</t>
   </si>
   <si>
@@ -253,18 +229,12 @@
     <t>Almiro Segóvia</t>
   </si>
   <si>
-    <t>Andreia, Filho, Filha</t>
-  </si>
-  <si>
     <t>Bruna</t>
   </si>
   <si>
     <t>Lucas</t>
   </si>
   <si>
-    <t>Jenifer, Filha</t>
-  </si>
-  <si>
     <t>Eduardo Rufino</t>
   </si>
   <si>
@@ -277,15 +247,9 @@
     <t>Cláudio</t>
   </si>
   <si>
-    <t>Cleysla</t>
-  </si>
-  <si>
     <t>Elaine</t>
   </si>
   <si>
-    <t>Marido</t>
-  </si>
-  <si>
     <t>Gustavo</t>
   </si>
   <si>
@@ -313,9 +277,6 @@
     <t>Arlei</t>
   </si>
   <si>
-    <t>Israel</t>
-  </si>
-  <si>
     <t>Rosana, Fernanda</t>
   </si>
   <si>
@@ -331,9 +292,6 @@
     <t>Juliana</t>
   </si>
   <si>
-    <t>Izadora</t>
-  </si>
-  <si>
     <t>Irani</t>
   </si>
   <si>
@@ -355,9 +313,6 @@
     <t>Tiago</t>
   </si>
   <si>
-    <t>Tais, Filhos</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -365,13 +320,112 @@
   </si>
   <si>
     <t>companions</t>
+  </si>
+  <si>
+    <t>Bruna, Filho, Filho</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Andreia, Lorena, Bernardo</t>
+  </si>
+  <si>
+    <t>Namorada</t>
+  </si>
+  <si>
+    <t>Cleysla, Vitor Hugo</t>
+  </si>
+  <si>
+    <t>Ismael</t>
+  </si>
+  <si>
+    <t>Daniel, Bia</t>
+  </si>
+  <si>
+    <t>Idalina, Gustavo</t>
+  </si>
+  <si>
+    <t>Luis Felipe</t>
+  </si>
+  <si>
+    <t>Celio, Guilherme, Leticia Eduarda</t>
+  </si>
+  <si>
+    <t>Elber Raul</t>
+  </si>
+  <si>
+    <t>Cida</t>
+  </si>
+  <si>
+    <t>Edroaldo</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Januário</t>
+  </si>
+  <si>
+    <t>Jenifer, Laura</t>
+  </si>
+  <si>
+    <t>Michele</t>
+  </si>
+  <si>
+    <t>Ana Clara, Davi Luis</t>
+  </si>
+  <si>
+    <t>Renato, Ana Julia, filho, filha</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Edivan</t>
+  </si>
+  <si>
+    <t>José Zito, filho, filho, filho</t>
+  </si>
+  <si>
+    <t>Luis Henrique</t>
+  </si>
+  <si>
+    <t>Wesley Cauã</t>
+  </si>
+  <si>
+    <t>Marinalva, Gabriel, Samuel, Vinicius, Agregada</t>
+  </si>
+  <si>
+    <t>agregado, agregado, agregado, agregado</t>
+  </si>
+  <si>
+    <t>agregado, agregado, agregado</t>
+  </si>
+  <si>
+    <t>Esposa, Valentina</t>
+  </si>
+  <si>
+    <t>Tais, Noah, Radasha</t>
+  </si>
+  <si>
+    <t>confirmation</t>
+  </si>
+  <si>
+    <t>Marido, Izadora, Lavinia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -382,6 +436,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -405,9 +473,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,30 +696,33 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,8 +732,11 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -670,8 +746,11 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -681,13 +760,16 @@
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -695,448 +777,667 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>67998288184</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="1" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="1" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="B21" s="1">
         <v>67998427540</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1">
         <v>67998309438</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23">
+        <v>67998283393</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="D26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B27">
+        <v>67998649667</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="B29">
+        <v>67999320791</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="B30">
+        <v>67996688193</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="B31">
+        <v>67999609548</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="B32">
+        <v>67998021616</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="1" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34">
+        <v>67998214020</v>
+      </c>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>67996583047</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39">
+        <v>67996535492</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43">
+        <v>67999008024</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B44">
+        <v>67996877988</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45">
+        <v>67999915759</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49">
+        <v>67999685021</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50">
+        <v>67998720526</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51">
+        <v>67993335825</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52">
+        <v>67999749660</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="1" t="s">
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="B54">
+        <v>67998948724</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="B55">
+        <v>67998577131</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="1" t="s">
+    </row>
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B56">
+        <v>67991475553</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B57">
+        <v>67981107189</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59">
+        <v>67998604034</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60">
+        <v>67998202294</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="D61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="B62">
+        <v>67999768984</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="1" t="s">
+    <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="D63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="B64">
+        <v>67996923269</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B65">
+        <v>67996679801</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66">
+        <v>67996754747</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="D67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="1" t="s">
+    </row>
+    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="B69">
+        <v>67999991812</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="B71">
+        <v>67998894695</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="B72">
+        <v>67992376409</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>111</v>
+      <c r="C73" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>